<commit_message>
#Ajuste el Burndown chart
</commit_message>
<xml_diff>
--- a/meetings/helpers/BurndownChart.20101018.xlsx
+++ b/meetings/helpers/BurndownChart.20101018.xlsx
@@ -298,24 +298,24 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88672512"/>
-        <c:axId val="88686592"/>
+        <c:axId val="79879168"/>
+        <c:axId val="80225024"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="88672512"/>
+        <c:axId val="79879168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,13 +333,13 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88686592"/>
+        <c:crossAx val="80225024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88686592"/>
+        <c:axId val="80225024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +376,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88672512"/>
+        <c:crossAx val="79879168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -385,7 +385,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -977,7 +977,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1143,7 +1143,7 @@
         <v>40466</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1151,7 +1151,7 @@
         <v>40467</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1159,7 +1159,7 @@
         <v>40468</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Burndown chart para el reporte de avance del 01/11/2010
</commit_message>
<xml_diff>
--- a/meetings/helpers/BurndownChart.20101018.xlsx
+++ b/meetings/helpers/BurndownChart.20101018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="270" windowWidth="19320" windowHeight="10680" activeTab="1"/>
+    <workbookView xWindow="840" yWindow="270" windowWidth="19320" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>completed</t>
   </si>
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t>Implementar la logica génerica de procesamiento de las metricas en base a los archivos de los sistemas externos usando la interfaz comun a todas</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -311,11 +305,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79879168"/>
-        <c:axId val="80225024"/>
+        <c:axId val="103559936"/>
+        <c:axId val="103561472"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="79879168"/>
+        <c:axId val="103559936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,13 +327,13 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80225024"/>
+        <c:crossAx val="103561472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="80225024"/>
+        <c:axId val="103561472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +370,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79879168"/>
+        <c:crossAx val="103559936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -385,7 +379,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -739,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -852,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -867,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -882,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -897,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -912,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -927,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -942,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ref="D13:D14" si="1">D12-B12</f>
@@ -957,7 +951,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="1"/>
@@ -976,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>